<commit_message>
Cargue en la base de datos v2
</commit_message>
<xml_diff>
--- a/atlas/ARCHIVO_EJEMPLO.xlsx
+++ b/atlas/ARCHIVO_EJEMPLO.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSITIES\UniBosque\PREGRADO 2021-2\PROYECTO NÚCLEO 2\PRIMER CORTE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\7° Semestre\Proyecto Nucleo 2\Corte 3\atlas\atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892E5063-6C8D-4538-8725-F299C462921A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NÓMINA" sheetId="1" r:id="rId1"/>
     <sheet name="PILA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NÓMINA!$A$6:$X$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NÓMINA!$A$6:$X$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>wilson.rojasreales@outlook.com</author>
   </authors>
   <commentList>
-    <comment ref="Y6" authorId="0" shapeId="0">
+    <comment ref="Y6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z6" authorId="0" shapeId="0">
+    <comment ref="Z6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>TIPO DOCUMENTO APORTANTE</t>
   </si>
@@ -187,9 +186,6 @@
   </si>
   <si>
     <t>F.INGRESO</t>
-  </si>
-  <si>
-    <t>dd/mm/aaaa</t>
   </si>
   <si>
     <t>INGRESO TOTAL</t>
@@ -258,7 +254,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,17 +335,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,6 +349,12 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,11 +668,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AD22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:AD7"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" topLeftCell="O5" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,15 +701,15 @@
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="AA2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" s="13">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="11">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="AC2" s="12">
+      <c r="AC2" s="10">
         <v>0.12</v>
       </c>
-      <c r="AD2" s="14">
+      <c r="AD2" s="12">
         <v>5.2199999999999998E-3</v>
       </c>
     </row>
@@ -734,12 +730,12 @@
         <v>23</v>
       </c>
       <c r="AA3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB3" s="12">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="10">
         <v>0.04</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AC3" s="10">
         <v>0.04</v>
       </c>
       <c r="AD3">
@@ -765,30 +761,30 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
-      <c r="O4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z4" s="8"/>
+      <c r="O4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z4" s="7"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -863,23 +859,23 @@
       <c r="X6" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA6" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB6" s="11" t="s">
+      <c r="Y6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AD6" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="AD6" s="11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -913,8 +909,8 @@
       <c r="L7">
         <v>30</v>
       </c>
-      <c r="M7" t="s">
-        <v>37</v>
+      <c r="M7" s="1">
+        <v>44540</v>
       </c>
       <c r="N7" s="4">
         <v>5000000</v>
@@ -970,706 +966,6 @@
       </c>
       <c r="AD7">
         <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8">
-        <v>9780</v>
-      </c>
-      <c r="F8">
-        <v>2017</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>23</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>5</v>
-      </c>
-      <c r="L8">
-        <v>30</v>
-      </c>
-      <c r="N8" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="O8" s="4">
-        <v>0</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>0</v>
-      </c>
-      <c r="R8" s="4">
-        <v>1686800</v>
-      </c>
-      <c r="S8" s="4">
-        <v>0</v>
-      </c>
-      <c r="T8" s="4">
-        <v>0</v>
-      </c>
-      <c r="U8" s="4">
-        <v>0</v>
-      </c>
-      <c r="V8" s="4">
-        <v>0</v>
-      </c>
-      <c r="W8" s="4">
-        <v>0</v>
-      </c>
-      <c r="X8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z8" s="4">
-        <f t="shared" ref="Z8:Z14" si="0">AA8-O8-V8-R8</f>
-        <v>4999000</v>
-      </c>
-      <c r="AA8" s="4">
-        <f t="shared" ref="AA8:AA14" si="1">SUM(N8:X8)-Y8</f>
-        <v>6685800</v>
-      </c>
-      <c r="AB8" s="4">
-        <f t="shared" ref="AB8:AC14" si="2">($Z$7*4)/100</f>
-        <v>208424.04</v>
-      </c>
-      <c r="AC8" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>9536</v>
-      </c>
-      <c r="F9">
-        <v>2017</v>
-      </c>
-      <c r="G9" s="5">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>30</v>
-      </c>
-      <c r="N9" s="4">
-        <v>5000000</v>
-      </c>
-      <c r="O9" s="4">
-        <v>0</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>0</v>
-      </c>
-      <c r="R9" s="4">
-        <v>3283226</v>
-      </c>
-      <c r="S9" s="4">
-        <v>0</v>
-      </c>
-      <c r="T9" s="4">
-        <v>0</v>
-      </c>
-      <c r="U9" s="4">
-        <v>0</v>
-      </c>
-      <c r="V9" s="4">
-        <v>7967445</v>
-      </c>
-      <c r="W9" s="4">
-        <v>0</v>
-      </c>
-      <c r="X9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z9" s="4">
-        <f t="shared" si="0"/>
-        <v>4999000</v>
-      </c>
-      <c r="AA9" s="4">
-        <f t="shared" si="1"/>
-        <v>16249671</v>
-      </c>
-      <c r="AB9" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AC9" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>9765</v>
-      </c>
-      <c r="F10">
-        <v>2017</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>30</v>
-      </c>
-      <c r="N10" s="4">
-        <v>7672257</v>
-      </c>
-      <c r="O10" s="4">
-        <v>0</v>
-      </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>0</v>
-      </c>
-      <c r="R10" s="4">
-        <v>0</v>
-      </c>
-      <c r="S10" s="4">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
-        <v>0</v>
-      </c>
-      <c r="U10" s="4">
-        <v>0</v>
-      </c>
-      <c r="V10" s="4">
-        <v>0</v>
-      </c>
-      <c r="W10" s="4">
-        <v>0</v>
-      </c>
-      <c r="X10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z10" s="4">
-        <f t="shared" si="0"/>
-        <v>7671257</v>
-      </c>
-      <c r="AA10" s="4">
-        <f t="shared" si="1"/>
-        <v>7671257</v>
-      </c>
-      <c r="AB10" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AC10" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>9396</v>
-      </c>
-      <c r="F11">
-        <v>2017</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-      <c r="N11" s="4">
-        <v>9270644</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0</v>
-      </c>
-      <c r="P11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>0</v>
-      </c>
-      <c r="R11" s="4">
-        <v>0</v>
-      </c>
-      <c r="S11" s="4">
-        <v>0</v>
-      </c>
-      <c r="T11" s="4">
-        <v>0</v>
-      </c>
-      <c r="U11" s="4">
-        <v>0</v>
-      </c>
-      <c r="V11" s="4">
-        <v>0</v>
-      </c>
-      <c r="W11" s="4">
-        <v>0</v>
-      </c>
-      <c r="X11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z11" s="4">
-        <f t="shared" si="0"/>
-        <v>9269644</v>
-      </c>
-      <c r="AA11" s="4">
-        <f t="shared" si="1"/>
-        <v>9269644</v>
-      </c>
-      <c r="AB11" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AC11" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12">
-        <v>9355</v>
-      </c>
-      <c r="F12">
-        <v>2017</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>30</v>
-      </c>
-      <c r="N12" s="4">
-        <v>9590321</v>
-      </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>0</v>
-      </c>
-      <c r="R12" s="4">
-        <v>0</v>
-      </c>
-      <c r="S12" s="4">
-        <v>0</v>
-      </c>
-      <c r="T12" s="4">
-        <v>0</v>
-      </c>
-      <c r="U12" s="4">
-        <v>0</v>
-      </c>
-      <c r="V12" s="4">
-        <v>0</v>
-      </c>
-      <c r="W12" s="4">
-        <v>0</v>
-      </c>
-      <c r="X12" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z12" s="4">
-        <f t="shared" si="0"/>
-        <v>9589321</v>
-      </c>
-      <c r="AA12" s="4">
-        <f t="shared" si="1"/>
-        <v>9589321</v>
-      </c>
-      <c r="AB12" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AC12" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>9372</v>
-      </c>
-      <c r="F13">
-        <v>2017</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>30</v>
-      </c>
-      <c r="N13" s="4">
-        <v>9590321</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>0</v>
-      </c>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4">
-        <v>0</v>
-      </c>
-      <c r="T13" s="4">
-        <v>0</v>
-      </c>
-      <c r="U13" s="4">
-        <v>0</v>
-      </c>
-      <c r="V13" s="4">
-        <v>0</v>
-      </c>
-      <c r="W13" s="4">
-        <v>0</v>
-      </c>
-      <c r="X13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z13" s="4">
-        <f t="shared" si="0"/>
-        <v>9589321</v>
-      </c>
-      <c r="AA13" s="4">
-        <f t="shared" si="1"/>
-        <v>9589321</v>
-      </c>
-      <c r="AB13" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AC13" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14">
-        <v>9374</v>
-      </c>
-      <c r="F14">
-        <v>2017</v>
-      </c>
-      <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>30</v>
-      </c>
-      <c r="N14" s="4">
-        <v>9590321</v>
-      </c>
-      <c r="O14" s="4">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>0</v>
-      </c>
-      <c r="R14" s="4">
-        <v>0</v>
-      </c>
-      <c r="S14" s="4">
-        <v>0</v>
-      </c>
-      <c r="T14" s="4">
-        <v>0</v>
-      </c>
-      <c r="U14" s="4">
-        <v>0</v>
-      </c>
-      <c r="V14" s="4">
-        <v>0</v>
-      </c>
-      <c r="W14" s="4">
-        <v>0</v>
-      </c>
-      <c r="X14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Z14" s="4">
-        <f t="shared" si="0"/>
-        <v>9589321</v>
-      </c>
-      <c r="AA14" s="4">
-        <f t="shared" si="1"/>
-        <v>9589321</v>
-      </c>
-      <c r="AB14" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AC14" s="4">
-        <f t="shared" si="2"/>
-        <v>208424.04</v>
-      </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15">
-        <v>875655</v>
-      </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15">
-        <v>2017</v>
-      </c>
-      <c r="G15" s="5">
-        <v>2</v>
-      </c>
-      <c r="L15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16">
-        <v>9780</v>
-      </c>
-      <c r="F16">
-        <v>2017</v>
-      </c>
-      <c r="G16" s="5">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>11</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17">
-        <v>9536</v>
-      </c>
-      <c r="F17">
-        <v>2017</v>
-      </c>
-      <c r="G17" s="5">
-        <v>2</v>
-      </c>
-      <c r="L17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18">
-        <v>9765</v>
-      </c>
-      <c r="F18">
-        <v>2017</v>
-      </c>
-      <c r="G18" s="5">
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>9396</v>
-      </c>
-      <c r="F19">
-        <v>2017</v>
-      </c>
-      <c r="G19" s="5">
-        <v>2</v>
-      </c>
-      <c r="L19">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>9355</v>
-      </c>
-      <c r="F20">
-        <v>2017</v>
-      </c>
-      <c r="G20" s="5">
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>9372</v>
-      </c>
-      <c r="F21">
-        <v>2017</v>
-      </c>
-      <c r="G21" s="5">
-        <v>2</v>
-      </c>
-      <c r="L21">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22">
-        <v>9374</v>
-      </c>
-      <c r="F22">
-        <v>2017</v>
-      </c>
-      <c r="G22" s="5">
-        <v>2</v>
-      </c>
-      <c r="L22">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1683,10 +979,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -1701,25 +997,25 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="7">
+        <v>45</v>
+      </c>
+      <c r="C2" s="6">
         <v>860098765</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="I2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -1728,57 +1024,57 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>875655</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>2017</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>55</v>
+      <c r="G4" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="H4" s="4">
         <v>5210601</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="13">
         <f>(H4*4)/100</f>
         <v>208424.04</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <v>0.04</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="13">
         <v>200000</v>
       </c>
       <c r="L4" s="4">
@@ -1786,36 +1082,36 @@
         <v>8424.0400000000081</v>
       </c>
       <c r="M4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>875655</v>
       </c>
       <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>2017</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>55</v>
+      <c r="G5" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="H5" s="4">
         <v>5210601</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="13">
         <f>(H5*4)/100</f>
         <v>208424.04</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="10">
         <v>0.04</v>
       </c>
       <c r="K5">
@@ -1826,36 +1122,36 @@
         <v>208424.04</v>
       </c>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>875655</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>2017</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>55</v>
+      <c r="G6" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="H6" s="4">
         <v>5210601</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="13">
         <f>(H6*4)/100</f>
         <v>208424.04</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="10">
         <v>0.04</v>
       </c>
       <c r="K6">
@@ -1866,7 +1162,7 @@
         <v>4.0000000008149073E-2</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>